<commit_message>
Modifiche finali 25 ago 25
</commit_message>
<xml_diff>
--- a/btp_dati.xlsx
+++ b/btp_dati.xlsx
@@ -479,7 +479,7 @@
         </is>
       </c>
       <c r="C2" t="n">
-        <v>106.19</v>
+        <v>106.1</v>
       </c>
       <c r="D2" t="n">
         <v>3.625</v>
@@ -502,7 +502,7 @@
         </is>
       </c>
       <c r="C3" t="n">
-        <v>109.25</v>
+        <v>109.11</v>
       </c>
       <c r="D3" t="n">
         <v>3.25</v>
@@ -525,7 +525,7 @@
         </is>
       </c>
       <c r="C4" t="n">
-        <v>111</v>
+        <v>110.61</v>
       </c>
       <c r="D4" t="n">
         <v>2.625</v>
@@ -548,7 +548,7 @@
         </is>
       </c>
       <c r="C5" t="n">
-        <v>116.87</v>
+        <v>116.49</v>
       </c>
       <c r="D5" t="n">
         <v>3</v>
@@ -571,7 +571,7 @@
         </is>
       </c>
       <c r="C6" t="n">
-        <v>117.2</v>
+        <v>116.8</v>
       </c>
       <c r="D6" t="n">
         <v>2.875</v>
@@ -594,7 +594,7 @@
         </is>
       </c>
       <c r="C7" t="n">
-        <v>112.81</v>
+        <v>112.38</v>
       </c>
       <c r="D7" t="n">
         <v>2.5</v>
@@ -617,7 +617,7 @@
         </is>
       </c>
       <c r="C8" t="n">
-        <v>107.17</v>
+        <v>106.79</v>
       </c>
       <c r="D8" t="n">
         <v>1.175</v>
@@ -640,7 +640,7 @@
         </is>
       </c>
       <c r="C9" t="n">
-        <v>103.72</v>
+        <v>103.19</v>
       </c>
       <c r="D9" t="n">
         <v>2</v>
@@ -663,7 +663,7 @@
         </is>
       </c>
       <c r="C10" t="n">
-        <v>112.55</v>
+        <v>111.95</v>
       </c>
       <c r="D10" t="n">
         <v>2.5</v>
@@ -686,7 +686,7 @@
         </is>
       </c>
       <c r="C11" t="n">
-        <v>112.37</v>
+        <v>111.73</v>
       </c>
       <c r="D11" t="n">
         <v>2.5</v>
@@ -709,7 +709,7 @@
         </is>
       </c>
       <c r="C12" t="n">
-        <v>106.15</v>
+        <v>105.4</v>
       </c>
       <c r="D12" t="n">
         <v>1.275</v>
@@ -732,7 +732,7 @@
         </is>
       </c>
       <c r="C13" t="n">
-        <v>101.271</v>
+        <v>101.253</v>
       </c>
       <c r="D13" t="n">
         <v>2.25</v>
@@ -754,6 +754,9 @@
           <t>Btpi-15st26 3,1%</t>
         </is>
       </c>
+      <c r="C14" t="n">
+        <v>102.86</v>
+      </c>
       <c r="D14" t="n">
         <v>1.55</v>
       </c>
@@ -795,7 +798,7 @@
         </is>
       </c>
       <c r="C16" t="n">
-        <v>95.56</v>
+        <v>95.47</v>
       </c>
       <c r="E16" t="inlineStr">
         <is>
@@ -815,7 +818,7 @@
         </is>
       </c>
       <c r="C17" t="n">
-        <v>90.41</v>
+        <v>90.22</v>
       </c>
       <c r="E17" t="inlineStr">
         <is>
@@ -835,7 +838,7 @@
         </is>
       </c>
       <c r="C18" t="n">
-        <v>85.2</v>
+        <v>85.25</v>
       </c>
       <c r="E18" t="inlineStr">
         <is>
@@ -906,7 +909,7 @@
         </is>
       </c>
       <c r="C22" t="n">
-        <v>107.07</v>
+        <v>106.87</v>
       </c>
       <c r="D22" t="n">
         <v>2.375</v>
@@ -929,7 +932,7 @@
         </is>
       </c>
       <c r="C23" t="n">
-        <v>108.62</v>
+        <v>107.85</v>
       </c>
       <c r="D23" t="n">
         <v>2.375</v>
@@ -952,7 +955,7 @@
         </is>
       </c>
       <c r="C24" t="n">
-        <v>93.42</v>
+        <v>93.37</v>
       </c>
       <c r="E24" t="inlineStr">
         <is>
@@ -972,7 +975,7 @@
         </is>
       </c>
       <c r="C25" t="n">
-        <v>89.26000000000001</v>
+        <v>89.06999999999999</v>
       </c>
       <c r="E25" t="inlineStr">
         <is>
@@ -1077,7 +1080,7 @@
         </is>
       </c>
       <c r="C31" t="n">
-        <v>104.05</v>
+        <v>103.78</v>
       </c>
       <c r="D31" t="n">
         <v>1.75</v>
@@ -1100,7 +1103,7 @@
         </is>
       </c>
       <c r="C32" t="n">
-        <v>87.2</v>
+        <v>86.51000000000001</v>
       </c>
       <c r="D32" t="n">
         <v>1.625</v>
@@ -1123,7 +1126,7 @@
         </is>
       </c>
       <c r="C33" t="n">
-        <v>92.29000000000001</v>
+        <v>91.97</v>
       </c>
       <c r="D33" t="n">
         <v>0.825</v>
@@ -1146,7 +1149,7 @@
         </is>
       </c>
       <c r="C34" t="n">
-        <v>100.01</v>
+        <v>100</v>
       </c>
       <c r="D34" t="n">
         <v>1</v>
@@ -1169,7 +1172,7 @@
         </is>
       </c>
       <c r="C35" t="n">
-        <v>100.03</v>
+        <v>99.70999999999999</v>
       </c>
       <c r="D35" t="n">
         <v>0.625</v>
@@ -1192,7 +1195,7 @@
         </is>
       </c>
       <c r="C36" t="n">
-        <v>79.23999999999999</v>
+        <v>78.51000000000001</v>
       </c>
       <c r="D36" t="n">
         <v>1.35</v>
@@ -1215,7 +1218,7 @@
         </is>
       </c>
       <c r="C37" t="n">
-        <v>99.736</v>
+        <v>99.729</v>
       </c>
       <c r="D37" t="n">
         <v>0.8</v>
@@ -1238,7 +1241,7 @@
         </is>
       </c>
       <c r="C38" t="n">
-        <v>88.06</v>
+        <v>87.58</v>
       </c>
       <c r="D38" t="n">
         <v>1.125</v>
@@ -1261,7 +1264,7 @@
         </is>
       </c>
       <c r="C39" t="n">
-        <v>99.14</v>
+        <v>99.06</v>
       </c>
       <c r="D39" t="n">
         <v>0.625</v>
@@ -1284,7 +1287,7 @@
         </is>
       </c>
       <c r="C40" t="n">
-        <v>69.83</v>
+        <v>69.11</v>
       </c>
       <c r="D40" t="n">
         <v>1.4</v>
@@ -1307,7 +1310,7 @@
         </is>
       </c>
       <c r="C41" t="n">
-        <v>94.81999999999999</v>
+        <v>94.31999999999999</v>
       </c>
       <c r="D41" t="n">
         <v>1.225</v>
@@ -1330,7 +1333,7 @@
         </is>
       </c>
       <c r="C42" t="n">
-        <v>100.27</v>
+        <v>100.2</v>
       </c>
       <c r="D42" t="n">
         <v>1.1</v>
@@ -1353,7 +1356,7 @@
         </is>
       </c>
       <c r="C43" t="n">
-        <v>101.19</v>
+        <v>101.25</v>
       </c>
       <c r="D43" t="n">
         <v>0.65</v>
@@ -1376,7 +1379,7 @@
         </is>
       </c>
       <c r="C44" t="n">
-        <v>89.09999999999999</v>
+        <v>88.43000000000001</v>
       </c>
       <c r="D44" t="n">
         <v>1.725</v>
@@ -1399,7 +1402,7 @@
         </is>
       </c>
       <c r="C45" t="n">
-        <v>99.95</v>
+        <v>99.87</v>
       </c>
       <c r="D45" t="n">
         <v>1.025</v>
@@ -1422,7 +1425,7 @@
         </is>
       </c>
       <c r="C46" t="n">
-        <v>91.7</v>
+        <v>91.18000000000001</v>
       </c>
       <c r="D46" t="n">
         <v>1.475</v>
@@ -1445,7 +1448,7 @@
         </is>
       </c>
       <c r="C47" t="n">
-        <v>99.56</v>
+        <v>99.54000000000001</v>
       </c>
       <c r="D47" t="n">
         <v>1</v>
@@ -1468,7 +1471,7 @@
         </is>
       </c>
       <c r="C48" t="n">
-        <v>99.836</v>
+        <v>99.84999999999999</v>
       </c>
       <c r="D48" t="n">
         <v>0.275</v>
@@ -1491,7 +1494,7 @@
         </is>
       </c>
       <c r="C49" t="n">
-        <v>101.55</v>
+        <v>101.43</v>
       </c>
       <c r="D49" t="n">
         <v>1.4</v>
@@ -1514,7 +1517,7 @@
         </is>
       </c>
       <c r="C50" t="n">
-        <v>100.099</v>
+        <v>100.078</v>
       </c>
       <c r="D50" t="n">
         <v>1.25</v>
@@ -1537,7 +1540,7 @@
         </is>
       </c>
       <c r="C51" t="n">
-        <v>99.7</v>
+        <v>99.19</v>
       </c>
       <c r="D51" t="n">
         <v>1.675</v>
@@ -1560,7 +1563,7 @@
         </is>
       </c>
       <c r="C52" t="n">
-        <v>94.25</v>
+        <v>93.5</v>
       </c>
       <c r="D52" t="n">
         <v>1.925</v>
@@ -1583,7 +1586,7 @@
         </is>
       </c>
       <c r="C53" t="n">
-        <v>102.06</v>
+        <v>101.85</v>
       </c>
       <c r="D53" t="n">
         <v>1.5</v>
@@ -1606,7 +1609,7 @@
         </is>
       </c>
       <c r="C54" t="n">
-        <v>100.1</v>
+        <v>100.071</v>
       </c>
       <c r="D54" t="n">
         <v>1.05</v>
@@ -1629,7 +1632,7 @@
         </is>
       </c>
       <c r="C55" t="n">
-        <v>91.33</v>
+        <v>90.73</v>
       </c>
       <c r="D55" t="n">
         <v>1.55</v>
@@ -1652,7 +1655,7 @@
         </is>
       </c>
       <c r="C56" t="n">
-        <v>94.66</v>
+        <v>94.45999999999999</v>
       </c>
       <c r="D56" t="n">
         <v>0.675</v>
@@ -1675,7 +1678,7 @@
         </is>
       </c>
       <c r="C57" t="n">
-        <v>97.23</v>
+        <v>97.12</v>
       </c>
       <c r="D57" t="n">
         <v>0.2</v>
@@ -1698,7 +1701,7 @@
         </is>
       </c>
       <c r="C58" t="n">
-        <v>99.81</v>
+        <v>99.79000000000001</v>
       </c>
       <c r="D58" t="n">
         <v>0.325</v>
@@ -1721,7 +1724,7 @@
         </is>
       </c>
       <c r="C59" t="n">
-        <v>98.45</v>
+        <v>98.5</v>
       </c>
       <c r="D59" t="n">
         <v>0.425</v>
@@ -1744,7 +1747,7 @@
         </is>
       </c>
       <c r="C60" t="n">
-        <v>72.22</v>
+        <v>71.67</v>
       </c>
       <c r="D60" t="n">
         <v>1.225</v>
@@ -1767,7 +1770,7 @@
         </is>
       </c>
       <c r="C61" t="n">
-        <v>81.69</v>
+        <v>81.27</v>
       </c>
       <c r="D61" t="n">
         <v>0.725</v>
@@ -1790,7 +1793,7 @@
         </is>
       </c>
       <c r="C62" t="n">
-        <v>92.09</v>
+        <v>91.86</v>
       </c>
       <c r="D62" t="n">
         <v>0.475</v>
@@ -1813,7 +1816,7 @@
         </is>
       </c>
       <c r="C63" t="n">
-        <v>94.66</v>
+        <v>94.40000000000001</v>
       </c>
       <c r="D63" t="n">
         <v>0.825</v>
@@ -1836,7 +1839,7 @@
         </is>
       </c>
       <c r="C64" t="n">
-        <v>93.94</v>
+        <v>93.7</v>
       </c>
       <c r="D64" t="n">
         <v>0.65</v>
@@ -1859,7 +1862,7 @@
         </is>
       </c>
       <c r="C65" t="n">
-        <v>99.59399999999999</v>
+        <v>99.521</v>
       </c>
       <c r="D65" t="n">
         <v>0.325</v>
@@ -1882,7 +1885,7 @@
         </is>
       </c>
       <c r="C66" t="n">
-        <v>97.72</v>
+        <v>97.65000000000001</v>
       </c>
       <c r="D66" t="n">
         <v>0.475</v>
@@ -1905,7 +1908,7 @@
         </is>
       </c>
       <c r="C67" t="n">
-        <v>99.364</v>
+        <v>99.348</v>
       </c>
       <c r="D67" t="n">
         <v>0.25</v>
@@ -1928,7 +1931,7 @@
         </is>
       </c>
       <c r="C68" t="n">
-        <v>74.98</v>
+        <v>74.48999999999999</v>
       </c>
       <c r="D68" t="n">
         <v>0.9</v>
@@ -1951,7 +1954,7 @@
         </is>
       </c>
       <c r="C69" t="n">
-        <v>90.17</v>
+        <v>89.90000000000001</v>
       </c>
       <c r="D69" t="n">
         <v>0.45</v>
@@ -1974,7 +1977,7 @@
         </is>
       </c>
       <c r="C70" t="n">
-        <v>60.43</v>
+        <v>59.88</v>
       </c>
       <c r="D70" t="n">
         <v>0.85</v>
@@ -1997,7 +2000,7 @@
         </is>
       </c>
       <c r="C71" t="n">
-        <v>95.23</v>
+        <v>95.26000000000001</v>
       </c>
       <c r="D71" t="n">
         <v>0.3</v>
@@ -2020,7 +2023,7 @@
         </is>
       </c>
       <c r="C72" t="n">
-        <v>74.78</v>
+        <v>74.34</v>
       </c>
       <c r="D72" t="n">
         <v>0.475</v>
@@ -2043,7 +2046,7 @@
         </is>
       </c>
       <c r="C73" t="n">
-        <v>95.20999999999999</v>
+        <v>95.08</v>
       </c>
       <c r="D73" t="n">
         <v>0.125</v>
@@ -2066,7 +2069,7 @@
         </is>
       </c>
       <c r="C74" t="n">
-        <v>87.73999999999999</v>
+        <v>87.47</v>
       </c>
       <c r="D74" t="n">
         <v>0.3</v>
@@ -2089,7 +2092,7 @@
         </is>
       </c>
       <c r="C75" t="n">
-        <v>58.73</v>
+        <v>58.13</v>
       </c>
       <c r="D75" t="n">
         <v>0.075</v>
@@ -2112,7 +2115,7 @@
         </is>
       </c>
       <c r="C76" t="n">
-        <v>98.84099999999999</v>
+        <v>98.821</v>
       </c>
       <c r="E76" t="inlineStr">
         <is>
@@ -2132,7 +2135,7 @@
         </is>
       </c>
       <c r="C77" t="n">
-        <v>65.26000000000001</v>
+        <v>64.72</v>
       </c>
       <c r="D77" t="n">
         <v>0.75</v>
@@ -2155,7 +2158,7 @@
         </is>
       </c>
       <c r="C78" t="n">
-        <v>57.49</v>
+        <v>56.85</v>
       </c>
       <c r="D78" t="n">
         <v>1.075</v>
@@ -2178,7 +2181,7 @@
         </is>
       </c>
       <c r="C79" t="n">
-        <v>79.09999999999999</v>
+        <v>78.77</v>
       </c>
       <c r="D79" t="n">
         <v>0.6</v>
@@ -2201,7 +2204,7 @@
         </is>
       </c>
       <c r="C80" t="n">
-        <v>95.13</v>
+        <v>94.98999999999999</v>
       </c>
       <c r="D80" t="n">
         <v>0.25</v>
@@ -2224,7 +2227,7 @@
         </is>
       </c>
       <c r="C81" t="n">
-        <v>88.78</v>
+        <v>88.48999999999999</v>
       </c>
       <c r="D81" t="n">
         <v>0.475</v>
@@ -2247,7 +2250,7 @@
         </is>
       </c>
       <c r="C82" t="n">
-        <v>98.29900000000001</v>
+        <v>98.268</v>
       </c>
       <c r="E82" t="inlineStr">
         <is>
@@ -2267,7 +2270,7 @@
         </is>
       </c>
       <c r="C83" t="n">
-        <v>87.54000000000001</v>
+        <v>87.19</v>
       </c>
       <c r="D83" t="n">
         <v>0.475</v>
@@ -2290,7 +2293,7 @@
         </is>
       </c>
       <c r="C84" t="n">
-        <v>87.3</v>
+        <v>86.91</v>
       </c>
       <c r="D84" t="n">
         <v>0.375</v>
@@ -2313,7 +2316,7 @@
         </is>
       </c>
       <c r="C85" t="n">
-        <v>93.62</v>
+        <v>93.5</v>
       </c>
       <c r="D85" t="n">
         <v>0.225</v>
@@ -2336,7 +2339,7 @@
         </is>
       </c>
       <c r="C86" t="n">
-        <v>66.05</v>
+        <v>65.47</v>
       </c>
       <c r="D86" t="n">
         <v>1.075</v>
@@ -2359,7 +2362,7 @@
         </is>
       </c>
       <c r="C87" t="n">
-        <v>90.02</v>
+        <v>89.70999999999999</v>
       </c>
       <c r="D87" t="n">
         <v>0.05</v>
@@ -2382,7 +2385,7 @@
         </is>
       </c>
       <c r="C88" t="n">
-        <v>98.53</v>
+        <v>98.45</v>
       </c>
       <c r="D88" t="n">
         <v>0.55</v>
@@ -2405,7 +2408,7 @@
         </is>
       </c>
       <c r="C89" t="n">
-        <v>96.19</v>
+        <v>95.81</v>
       </c>
       <c r="D89" t="n">
         <v>1.25</v>
@@ -2428,7 +2431,7 @@
         </is>
       </c>
       <c r="C90" t="n">
-        <v>101.19</v>
+        <v>101.01</v>
       </c>
       <c r="D90" t="n">
         <v>1.4</v>
@@ -2451,7 +2454,7 @@
         </is>
       </c>
       <c r="C91" t="n">
-        <v>95.06999999999999</v>
+        <v>94.5</v>
       </c>
       <c r="D91" t="n">
         <v>1.625</v>
@@ -2474,7 +2477,7 @@
         </is>
       </c>
       <c r="C92" t="n">
-        <v>100.86</v>
+        <v>100.8</v>
       </c>
       <c r="D92" t="n">
         <v>0.8</v>
@@ -2633,7 +2636,7 @@
         </is>
       </c>
       <c r="C101" t="n">
-        <v>101.05</v>
+        <v>100.91</v>
       </c>
       <c r="D101" t="n">
         <v>1.325</v>
@@ -2656,7 +2659,7 @@
         </is>
       </c>
       <c r="C102" t="n">
-        <v>105.27</v>
+        <v>104.77</v>
       </c>
       <c r="D102" t="n">
         <v>2</v>
@@ -2679,7 +2682,7 @@
         </is>
       </c>
       <c r="C103" t="n">
-        <v>100.549</v>
+        <v>100.544</v>
       </c>
       <c r="D103" t="n">
         <v>1.75</v>
@@ -2702,7 +2705,7 @@
         </is>
       </c>
       <c r="C104" t="n">
-        <v>101.51</v>
+        <v>101.42</v>
       </c>
       <c r="D104" t="n">
         <v>0.8</v>
@@ -2725,7 +2728,7 @@
         </is>
       </c>
       <c r="C105" t="n">
-        <v>108.37</v>
+        <v>107.99</v>
       </c>
       <c r="D105" t="n">
         <v>2.2</v>
@@ -2748,7 +2751,7 @@
         </is>
       </c>
       <c r="C106" t="n">
-        <v>105.11</v>
+        <v>104.88</v>
       </c>
       <c r="D106" t="n">
         <v>1.925</v>
@@ -2771,7 +2774,7 @@
         </is>
       </c>
       <c r="C107" t="n">
-        <v>102.89</v>
+        <v>102.78</v>
       </c>
       <c r="D107" t="n">
         <v>1.7</v>
@@ -2811,7 +2814,7 @@
         </is>
       </c>
       <c r="C109" t="n">
-        <v>104.33</v>
+        <v>103.69</v>
       </c>
       <c r="D109" t="n">
         <v>2.225</v>
@@ -2834,7 +2837,7 @@
         </is>
       </c>
       <c r="C110" t="n">
-        <v>102.43</v>
+        <v>102.34</v>
       </c>
       <c r="D110" t="n">
         <v>1</v>
@@ -2857,7 +2860,7 @@
         </is>
       </c>
       <c r="C111" t="n">
-        <v>101.48</v>
+        <v>100.63</v>
       </c>
       <c r="D111" t="n">
         <v>2.25</v>
@@ -2880,7 +2883,7 @@
         </is>
       </c>
       <c r="C112" t="n">
-        <v>101.126</v>
+        <v>101.11</v>
       </c>
       <c r="D112" t="n">
         <v>1.9</v>
@@ -2903,7 +2906,7 @@
         </is>
       </c>
       <c r="C113" t="n">
-        <v>106.27</v>
+        <v>106.02</v>
       </c>
       <c r="D113" t="n">
         <v>2</v>
@@ -2926,7 +2929,7 @@
         </is>
       </c>
       <c r="C114" t="n">
-        <v>104.53</v>
+        <v>104.28</v>
       </c>
       <c r="D114" t="n">
         <v>1.85</v>
@@ -2948,9 +2951,6 @@
           <t>Btpi Tf 1.5% Mg29 Eur</t>
         </is>
       </c>
-      <c r="C115" t="n">
-        <v>101.9</v>
-      </c>
       <c r="D115" t="n">
         <v>0.75</v>
       </c>
@@ -2972,7 +2972,7 @@
         </is>
       </c>
       <c r="C116" t="n">
-        <v>107.84</v>
+        <v>107.39</v>
       </c>
       <c r="D116" t="n">
         <v>2.175</v>
@@ -2995,7 +2995,7 @@
         </is>
       </c>
       <c r="C117" t="n">
-        <v>102.95</v>
+        <v>102.81</v>
       </c>
       <c r="D117" t="n">
         <v>2</v>
@@ -3018,7 +3018,7 @@
         </is>
       </c>
       <c r="C118" t="n">
-        <v>103.1</v>
+        <v>102.68</v>
       </c>
       <c r="D118" t="n">
         <v>1.2</v>
@@ -3041,7 +3041,7 @@
         </is>
       </c>
       <c r="C119" t="n">
-        <v>104.19</v>
+        <v>104.04</v>
       </c>
       <c r="D119" t="n">
         <v>1.9</v>
@@ -3081,7 +3081,7 @@
         </is>
       </c>
       <c r="C121" t="n">
-        <v>101.86</v>
+        <v>101.79</v>
       </c>
       <c r="D121" t="n">
         <v>1.925</v>
@@ -3104,7 +3104,7 @@
         </is>
       </c>
       <c r="C122" t="n">
-        <v>100.144</v>
+        <v>100.15</v>
       </c>
       <c r="D122" t="n">
         <v>1.8</v>
@@ -3127,7 +3127,7 @@
         </is>
       </c>
       <c r="C123" t="n">
-        <v>106.64</v>
+        <v>106.17</v>
       </c>
       <c r="D123" t="n">
         <v>2.1</v>
@@ -3150,7 +3150,7 @@
         </is>
       </c>
       <c r="C124" t="n">
-        <v>105.92</v>
+        <v>105.61</v>
       </c>
       <c r="D124" t="n">
         <v>2</v>
@@ -3173,7 +3173,7 @@
         </is>
       </c>
       <c r="C125" t="n">
-        <v>105.45</v>
+        <v>105.17</v>
       </c>
       <c r="D125" t="n">
         <v>1.025</v>
@@ -3196,7 +3196,7 @@
         </is>
       </c>
       <c r="C126" t="n">
-        <v>105.47</v>
+        <v>105.28</v>
       </c>
       <c r="E126" t="inlineStr">
         <is>
@@ -3216,7 +3216,7 @@
         </is>
       </c>
       <c r="C127" t="n">
-        <v>101.17</v>
+        <v>101.14</v>
       </c>
       <c r="D127" t="n">
         <v>1.475</v>
@@ -3239,7 +3239,7 @@
         </is>
       </c>
       <c r="C128" t="n">
-        <v>103.34</v>
+        <v>103.06</v>
       </c>
       <c r="D128" t="n">
         <v>1.75</v>
@@ -3262,7 +3262,7 @@
         </is>
       </c>
       <c r="C129" t="n">
-        <v>102.95</v>
+        <v>102.28</v>
       </c>
       <c r="E129" t="inlineStr">
         <is>
@@ -3282,7 +3282,7 @@
         </is>
       </c>
       <c r="C130" t="n">
-        <v>103.78</v>
+        <v>103.55</v>
       </c>
       <c r="D130" t="n">
         <v>0.8125</v>
@@ -3305,7 +3305,7 @@
         </is>
       </c>
       <c r="C131" t="n">
-        <v>100.491</v>
+        <v>100.467</v>
       </c>
       <c r="D131" t="n">
         <v>1.6</v>
@@ -3328,7 +3328,7 @@
         </is>
       </c>
       <c r="C132" t="n">
-        <v>103.01</v>
+        <v>102.81</v>
       </c>
       <c r="D132" t="n">
         <v>1.675</v>
@@ -3351,7 +3351,7 @@
         </is>
       </c>
       <c r="C133" t="n">
-        <v>103.81</v>
+        <v>103.38</v>
       </c>
       <c r="D133" t="n">
         <v>1.925</v>
@@ -3374,7 +3374,7 @@
         </is>
       </c>
       <c r="C134" t="n">
-        <v>98.98</v>
+        <v>98.7</v>
       </c>
       <c r="D134" t="n">
         <v>0.9</v>
@@ -3397,7 +3397,7 @@
         </is>
       </c>
       <c r="C135" t="n">
-        <v>103.7</v>
+        <v>103.36</v>
       </c>
       <c r="D135" t="n">
         <v>0.8375</v>
@@ -3420,7 +3420,7 @@
         </is>
       </c>
       <c r="C136" t="n">
-        <v>102.91</v>
+        <v>102.64</v>
       </c>
       <c r="D136" t="n">
         <v>1.725</v>
@@ -3443,7 +3443,7 @@
         </is>
       </c>
       <c r="C137" t="n">
-        <v>103.44</v>
+        <v>102.86</v>
       </c>
       <c r="D137" t="n">
         <v>2.025</v>
@@ -3466,7 +3466,7 @@
         </is>
       </c>
       <c r="C138" t="n">
-        <v>102.31</v>
+        <v>102.28</v>
       </c>
       <c r="D138" t="n">
         <v>1.725</v>
@@ -3489,7 +3489,7 @@
         </is>
       </c>
       <c r="C139" t="n">
-        <v>101.06</v>
+        <v>101</v>
       </c>
       <c r="D139" t="n">
         <v>1.55</v>
@@ -3512,7 +3512,7 @@
         </is>
       </c>
       <c r="C140" t="n">
-        <v>103.36</v>
+        <v>102.9</v>
       </c>
       <c r="D140" t="n">
         <v>1.925</v>
@@ -3535,7 +3535,7 @@
         </is>
       </c>
       <c r="C141" t="n">
-        <v>101.68</v>
+        <v>101.48</v>
       </c>
       <c r="D141" t="n">
         <v>1.5</v>
@@ -3558,7 +3558,7 @@
         </is>
       </c>
       <c r="C142" t="n">
-        <v>97.62</v>
+        <v>96.84999999999999</v>
       </c>
       <c r="D142" t="n">
         <v>2.15</v>
@@ -3581,7 +3581,7 @@
         </is>
       </c>
       <c r="C143" t="n">
-        <v>101.04</v>
+        <v>100.71</v>
       </c>
       <c r="D143" t="n">
         <v>1.575</v>
@@ -3604,7 +3604,7 @@
         </is>
       </c>
       <c r="C144" t="n">
-        <v>100.11</v>
+        <v>100.97</v>
       </c>
       <c r="D144" t="n">
         <v>1.35</v>
@@ -3627,7 +3627,7 @@
         </is>
       </c>
       <c r="C145" t="n">
-        <v>101.29</v>
+        <v>100.78</v>
       </c>
       <c r="D145" t="n">
         <v>1.825</v>
@@ -3650,7 +3650,7 @@
         </is>
       </c>
       <c r="C146" t="n">
-        <v>99.39</v>
+        <v>98.7</v>
       </c>
       <c r="D146" t="n">
         <v>2.05</v>
@@ -3673,7 +3673,7 @@
         </is>
       </c>
       <c r="C147" t="n">
-        <v>100.59</v>
+        <v>100.58</v>
       </c>
       <c r="D147" t="n">
         <v>1.275</v>
@@ -3696,7 +3696,7 @@
         </is>
       </c>
       <c r="C148" t="n">
-        <v>100.77</v>
+        <v>100.44</v>
       </c>
       <c r="D148" t="n">
         <v>0.7125</v>
@@ -3719,7 +3719,7 @@
         </is>
       </c>
       <c r="C149" t="n">
-        <v>98.66</v>
+        <v>98.08</v>
       </c>
       <c r="D149" t="n">
         <v>1.925</v>
@@ -3742,7 +3742,7 @@
         </is>
       </c>
       <c r="C150" t="n">
-        <v>100.91</v>
+        <v>100.82</v>
       </c>
       <c r="D150" t="n">
         <v>1.475</v>
@@ -3765,7 +3765,7 @@
         </is>
       </c>
       <c r="C151" t="n">
-        <v>100.83</v>
+        <v>100.81</v>
       </c>
       <c r="D151" t="n">
         <v>1.325</v>
@@ -3788,7 +3788,7 @@
         </is>
       </c>
       <c r="C152" t="n">
-        <v>100.94</v>
+        <v>100.69</v>
       </c>
       <c r="D152" t="n">
         <v>1.625</v>
@@ -3811,7 +3811,7 @@
         </is>
       </c>
       <c r="C153" t="n">
-        <v>98.38</v>
+        <v>97.3</v>
       </c>
       <c r="D153" t="n">
         <v>1.275</v>
@@ -3834,7 +3834,7 @@
         </is>
       </c>
       <c r="C154" t="n">
-        <v>100.64</v>
+        <v>100.18</v>
       </c>
       <c r="D154" t="n">
         <v>1.49508</v>
@@ -3857,7 +3857,7 @@
         </is>
       </c>
       <c r="C155" t="n">
-        <v>100.47</v>
+        <v>100.29</v>
       </c>
       <c r="D155" t="n">
         <v>0.925</v>
@@ -3880,7 +3880,7 @@
         </is>
       </c>
       <c r="C156" t="n">
-        <v>99.69</v>
+        <v>99.40000000000001</v>
       </c>
       <c r="D156" t="n">
         <v>0.82623</v>
@@ -3903,7 +3903,7 @@
         </is>
       </c>
       <c r="C157" t="n">
-        <v>99.94</v>
+        <v>99.93000000000001</v>
       </c>
       <c r="D157" t="n">
         <v>0.34807</v>
@@ -3926,7 +3926,7 @@
         </is>
       </c>
       <c r="C158" t="n">
-        <v>99.38</v>
+        <v>99.36</v>
       </c>
       <c r="D158" t="n">
         <v>0.55</v>
@@ -3949,7 +3949,7 @@
         </is>
       </c>
       <c r="C159" t="n">
-        <v>99.75</v>
+        <v>99.56</v>
       </c>
       <c r="D159" t="n">
         <v>1.175</v>

</xml_diff>